<commit_message>
Allow ExcelReader to deal with multiple sheets and include tests and test data for this scenario
</commit_message>
<xml_diff>
--- a/thirdparty_loads/src/test/resources/threei/tempAna.xlsx
+++ b/thirdparty_loads/src/test/resources/threei/tempAna.xlsx
@@ -381,14 +381,14 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="K1" activeCellId="0" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K1" activeCellId="0" sqref="K1"/>
+      <selection pane="bottomRight" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="12" min="1" style="0" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="32"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="12" min="1" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="31.5867346938776"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="13.9030612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>